<commit_message>
new highlights figure from all exp
</commit_message>
<xml_diff>
--- a/results/correctnessExp2.xlsx
+++ b/results/correctnessExp2.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\agentSummaryUserStudy\results\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="420" windowWidth="19875" windowHeight="6690"/>
+    <workbookView xWindow="360" yWindow="420" windowWidth="19880" windowHeight="6690"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -180,12 +185,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -222,6 +227,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -270,7 +278,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -305,7 +313,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -517,12 +525,12 @@
   <dimension ref="A1:L343"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:L343"/>
+      <selection activeCell="I2" sqref="A1:L343"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -560,7 +568,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -602,7 +610,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -644,7 +652,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -686,7 +694,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -728,7 +736,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -770,7 +778,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -812,7 +820,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -854,7 +862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -896,7 +904,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -938,7 +946,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -980,7 +988,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -1022,7 +1030,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -1064,7 +1072,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1106,7 +1114,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1148,7 +1156,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -1190,7 +1198,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1232,7 +1240,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -1274,7 +1282,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1316,7 +1324,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>14</v>
       </c>
@@ -1358,7 +1366,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -1400,7 +1408,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>14</v>
       </c>
@@ -1442,7 +1450,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>14</v>
       </c>
@@ -1484,7 +1492,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>20</v>
       </c>
@@ -1526,7 +1534,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>12</v>
       </c>
@@ -1568,7 +1576,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>19</v>
       </c>
@@ -1610,7 +1618,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>18</v>
       </c>
@@ -1652,7 +1660,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>21</v>
       </c>
@@ -1694,7 +1702,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>16</v>
       </c>
@@ -1736,7 +1744,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>14</v>
       </c>
@@ -1778,7 +1786,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>22</v>
       </c>
@@ -1820,7 +1828,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>14</v>
       </c>
@@ -1862,7 +1870,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>12</v>
       </c>
@@ -1904,7 +1912,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>20</v>
       </c>
@@ -1946,7 +1954,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>19</v>
       </c>
@@ -1988,7 +1996,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>18</v>
       </c>
@@ -2030,7 +2038,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>20</v>
       </c>
@@ -2072,7 +2080,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>19</v>
       </c>
@@ -2114,7 +2122,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>16</v>
       </c>
@@ -2156,7 +2164,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>21</v>
       </c>
@@ -2198,7 +2206,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>20</v>
       </c>
@@ -2240,7 +2248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>19</v>
       </c>
@@ -2282,7 +2290,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>18</v>
       </c>
@@ -2324,7 +2332,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>22</v>
       </c>
@@ -2366,7 +2374,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>12</v>
       </c>
@@ -2408,7 +2416,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>23</v>
       </c>
@@ -2450,7 +2458,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>20</v>
       </c>
@@ -2492,7 +2500,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>16</v>
       </c>
@@ -2534,7 +2542,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>19</v>
       </c>
@@ -2576,7 +2584,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>21</v>
       </c>
@@ -2618,7 +2626,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>18</v>
       </c>
@@ -2660,7 +2668,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>24</v>
       </c>
@@ -2702,7 +2710,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>25</v>
       </c>
@@ -2744,7 +2752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>12</v>
       </c>
@@ -2786,7 +2794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>20</v>
       </c>
@@ -2828,7 +2836,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>21</v>
       </c>
@@ -2870,7 +2878,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>18</v>
       </c>
@@ -2912,7 +2920,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>19</v>
       </c>
@@ -2954,7 +2962,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>26</v>
       </c>
@@ -2996,7 +3004,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>16</v>
       </c>
@@ -3038,7 +3046,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>23</v>
       </c>
@@ -3080,7 +3088,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>22</v>
       </c>
@@ -3122,7 +3130,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>12</v>
       </c>
@@ -3164,7 +3172,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>21</v>
       </c>
@@ -3206,7 +3214,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>25</v>
       </c>
@@ -3248,7 +3256,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>18</v>
       </c>
@@ -3290,7 +3298,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>26</v>
       </c>
@@ -3332,7 +3340,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>12</v>
       </c>
@@ -3374,7 +3382,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>23</v>
       </c>
@@ -3416,7 +3424,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>16</v>
       </c>
@@ -3458,7 +3466,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>24</v>
       </c>
@@ -3500,7 +3508,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>21</v>
       </c>
@@ -3542,7 +3550,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>23</v>
       </c>
@@ -3584,7 +3592,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>12</v>
       </c>
@@ -3626,7 +3634,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>22</v>
       </c>
@@ -3668,7 +3676,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>16</v>
       </c>
@@ -3710,7 +3718,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>26</v>
       </c>
@@ -3752,7 +3760,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>21</v>
       </c>
@@ -3794,7 +3802,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>23</v>
       </c>
@@ -3836,7 +3844,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>25</v>
       </c>
@@ -3878,7 +3886,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>26</v>
       </c>
@@ -3920,7 +3928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>24</v>
       </c>
@@ -3962,7 +3970,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>26</v>
       </c>
@@ -4004,7 +4012,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>21</v>
       </c>
@@ -4046,7 +4054,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>23</v>
       </c>
@@ -4088,7 +4096,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>27</v>
       </c>
@@ -4130,7 +4138,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>26</v>
       </c>
@@ -4172,7 +4180,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>25</v>
       </c>
@@ -4214,7 +4222,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>23</v>
       </c>
@@ -4256,7 +4264,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>28</v>
       </c>
@@ -4298,7 +4306,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>22</v>
       </c>
@@ -4340,7 +4348,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>27</v>
       </c>
@@ -4382,7 +4390,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>26</v>
       </c>
@@ -4424,7 +4432,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>24</v>
       </c>
@@ -4466,7 +4474,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>23</v>
       </c>
@@ -4508,7 +4516,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>25</v>
       </c>
@@ -4550,7 +4558,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>27</v>
       </c>
@@ -4592,7 +4600,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>26</v>
       </c>
@@ -4634,7 +4642,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>28</v>
       </c>
@@ -4676,7 +4684,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>22</v>
       </c>
@@ -4718,7 +4726,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>23</v>
       </c>
@@ -4760,7 +4768,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>29</v>
       </c>
@@ -4802,7 +4810,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>30</v>
       </c>
@@ -4844,7 +4852,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>30</v>
       </c>
@@ -4886,7 +4894,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>31</v>
       </c>
@@ -4928,7 +4936,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>26</v>
       </c>
@@ -4970,7 +4978,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>30</v>
       </c>
@@ -5012,7 +5020,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>27</v>
       </c>
@@ -5054,7 +5062,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>30</v>
       </c>
@@ -5096,7 +5104,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>24</v>
       </c>
@@ -5138,7 +5146,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>30</v>
       </c>
@@ -5180,7 +5188,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>25</v>
       </c>
@@ -5222,7 +5230,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>30</v>
       </c>
@@ -5264,7 +5272,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>28</v>
       </c>
@@ -5306,7 +5314,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>30</v>
       </c>
@@ -5348,7 +5356,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>29</v>
       </c>
@@ -5390,7 +5398,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>30</v>
       </c>
@@ -5432,7 +5440,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>30</v>
       </c>
@@ -5474,7 +5482,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>27</v>
       </c>
@@ -5516,7 +5524,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>22</v>
       </c>
@@ -5558,7 +5566,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>28</v>
       </c>
@@ -5600,7 +5608,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>31</v>
       </c>
@@ -5642,7 +5650,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>27</v>
       </c>
@@ -5684,7 +5692,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>32</v>
       </c>
@@ -5726,7 +5734,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>24</v>
       </c>
@@ -5768,7 +5776,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>25</v>
       </c>
@@ -5810,7 +5818,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>32</v>
       </c>
@@ -5852,7 +5860,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>29</v>
       </c>
@@ -5894,7 +5902,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>27</v>
       </c>
@@ -5936,7 +5944,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>31</v>
       </c>
@@ -5978,7 +5986,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>32</v>
       </c>
@@ -6020,7 +6028,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>28</v>
       </c>
@@ -6062,7 +6070,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>24</v>
       </c>
@@ -6104,7 +6112,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>22</v>
       </c>
@@ -6146,7 +6154,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>27</v>
       </c>
@@ -6188,7 +6196,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>25</v>
       </c>
@@ -6230,7 +6238,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>29</v>
       </c>
@@ -6272,7 +6280,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>32</v>
       </c>
@@ -6314,7 +6322,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>27</v>
       </c>
@@ -6356,7 +6364,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>24</v>
       </c>
@@ -6398,7 +6406,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>31</v>
       </c>
@@ -6440,7 +6448,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>28</v>
       </c>
@@ -6482,7 +6490,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>32</v>
       </c>
@@ -6524,7 +6532,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>29</v>
       </c>
@@ -6566,7 +6574,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>32</v>
       </c>
@@ -6608,7 +6616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>25</v>
       </c>
@@ -6650,7 +6658,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>32</v>
       </c>
@@ -6692,7 +6700,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>22</v>
       </c>
@@ -6734,7 +6742,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>28</v>
       </c>
@@ -6776,7 +6784,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>32</v>
       </c>
@@ -6818,7 +6826,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>31</v>
       </c>
@@ -6860,7 +6868,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="152" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>29</v>
       </c>
@@ -6902,7 +6910,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>24</v>
       </c>
@@ -6944,7 +6952,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>32</v>
       </c>
@@ -6986,7 +6994,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>29</v>
       </c>
@@ -7028,7 +7036,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="156" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>28</v>
       </c>
@@ -7070,7 +7078,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>31</v>
       </c>
@@ -7112,7 +7120,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>28</v>
       </c>
@@ -7154,7 +7162,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>29</v>
       </c>
@@ -7196,7 +7204,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="160" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>31</v>
       </c>
@@ -7238,7 +7246,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>31</v>
       </c>
@@ -7280,7 +7288,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="162" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>31</v>
       </c>
@@ -7322,7 +7330,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>29</v>
       </c>
@@ -7364,7 +7372,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="164" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>33</v>
       </c>
@@ -7406,7 +7414,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>34</v>
       </c>
@@ -7448,7 +7456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>33</v>
       </c>
@@ -7490,7 +7498,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>35</v>
       </c>
@@ -7532,7 +7540,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>34</v>
       </c>
@@ -7574,7 +7582,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>35</v>
       </c>
@@ -7616,7 +7624,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="170" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>36</v>
       </c>
@@ -7658,7 +7666,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>34</v>
       </c>
@@ -7700,7 +7708,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="172" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>37</v>
       </c>
@@ -7742,7 +7750,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="173" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>35</v>
       </c>
@@ -7784,7 +7792,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="174" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>33</v>
       </c>
@@ -7826,7 +7834,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="175" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>34</v>
       </c>
@@ -7868,7 +7876,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="176" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>38</v>
       </c>
@@ -7910,7 +7918,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="177" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>36</v>
       </c>
@@ -7952,7 +7960,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="178" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>37</v>
       </c>
@@ -7994,7 +8002,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="179" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>35</v>
       </c>
@@ -8036,7 +8044,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="180" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>35</v>
       </c>
@@ -8078,7 +8086,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="181" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>34</v>
       </c>
@@ -8120,7 +8128,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="182" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>37</v>
       </c>
@@ -8162,7 +8170,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>36</v>
       </c>
@@ -8204,7 +8212,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="184" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>35</v>
       </c>
@@ -8246,7 +8254,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="185" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>37</v>
       </c>
@@ -8288,7 +8296,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="186" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>34</v>
       </c>
@@ -8330,7 +8338,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="187" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>35</v>
       </c>
@@ -8372,7 +8380,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="188" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>36</v>
       </c>
@@ -8414,7 +8422,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="189" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>34</v>
       </c>
@@ -8456,7 +8464,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="190" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>37</v>
       </c>
@@ -8498,7 +8506,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="191" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>35</v>
       </c>
@@ -8540,7 +8548,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="192" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>34</v>
       </c>
@@ -8582,7 +8590,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="193" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>33</v>
       </c>
@@ -8624,7 +8632,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="194" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>37</v>
       </c>
@@ -8666,7 +8674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>35</v>
       </c>
@@ -8708,7 +8716,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="196" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>38</v>
       </c>
@@ -8750,7 +8758,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="197" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>34</v>
       </c>
@@ -8792,7 +8800,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="198" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>36</v>
       </c>
@@ -8834,7 +8842,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="199" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>37</v>
       </c>
@@ -8876,7 +8884,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="200" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>36</v>
       </c>
@@ -8918,7 +8926,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="201" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>37</v>
       </c>
@@ -8960,7 +8968,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="202" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>37</v>
       </c>
@@ -9002,7 +9010,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="203" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>36</v>
       </c>
@@ -9044,7 +9052,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="204" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>33</v>
       </c>
@@ -9086,7 +9094,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="205" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>39</v>
       </c>
@@ -9128,7 +9136,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="206" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>36</v>
       </c>
@@ -9170,7 +9178,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="207" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>39</v>
       </c>
@@ -9212,7 +9220,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="208" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>38</v>
       </c>
@@ -9254,7 +9262,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="209" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>39</v>
       </c>
@@ -9296,7 +9304,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="210" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>33</v>
       </c>
@@ -9338,7 +9346,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="211" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>36</v>
       </c>
@@ -9380,7 +9388,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="212" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>39</v>
       </c>
@@ -9422,7 +9430,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="213" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>39</v>
       </c>
@@ -9464,7 +9472,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="214" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>39</v>
       </c>
@@ -9506,7 +9514,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="215" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>33</v>
       </c>
@@ -9548,7 +9556,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="216" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>39</v>
       </c>
@@ -9590,7 +9598,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="217" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>40</v>
       </c>
@@ -9632,7 +9640,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="218" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>39</v>
       </c>
@@ -9674,7 +9682,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="219" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>33</v>
       </c>
@@ -9716,7 +9724,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="220" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>39</v>
       </c>
@@ -9758,7 +9766,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="221" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>40</v>
       </c>
@@ -9800,7 +9808,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="222" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>38</v>
       </c>
@@ -9842,7 +9850,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="223" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>33</v>
       </c>
@@ -9884,7 +9892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="224" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>41</v>
       </c>
@@ -9926,7 +9934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="225" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>40</v>
       </c>
@@ -9968,7 +9976,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="226" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
         <v>40</v>
       </c>
@@ -10010,7 +10018,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="227" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
         <v>40</v>
       </c>
@@ -10052,7 +10060,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="228" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>38</v>
       </c>
@@ -10094,7 +10102,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="229" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
         <v>41</v>
       </c>
@@ -10136,7 +10144,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="230" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
         <v>40</v>
       </c>
@@ -10178,7 +10186,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="231" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
         <v>40</v>
       </c>
@@ -10220,7 +10228,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="232" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
         <v>42</v>
       </c>
@@ -10262,7 +10270,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="233" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
         <v>38</v>
       </c>
@@ -10304,7 +10312,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="234" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
         <v>40</v>
       </c>
@@ -10346,7 +10354,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="235" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
         <v>40</v>
       </c>
@@ -10388,7 +10396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="236" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
         <v>43</v>
       </c>
@@ -10430,7 +10438,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="237" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
         <v>42</v>
       </c>
@@ -10472,7 +10480,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="238" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
         <v>44</v>
       </c>
@@ -10514,7 +10522,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="239" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A239" s="1" t="s">
         <v>45</v>
       </c>
@@ -10556,7 +10564,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="240" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
         <v>41</v>
       </c>
@@ -10598,7 +10606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="241" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
         <v>43</v>
       </c>
@@ -10640,7 +10648,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="242" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
         <v>38</v>
       </c>
@@ -10682,7 +10690,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="243" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A243" s="1" t="s">
         <v>45</v>
       </c>
@@ -10724,7 +10732,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="244" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
         <v>42</v>
       </c>
@@ -10766,7 +10774,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="245" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
         <v>44</v>
       </c>
@@ -10808,7 +10816,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="246" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
         <v>41</v>
       </c>
@@ -10850,7 +10858,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="247" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
         <v>43</v>
       </c>
@@ -10892,7 +10900,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="248" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A248" s="1" t="s">
         <v>45</v>
       </c>
@@ -10934,7 +10942,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="249" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
         <v>44</v>
       </c>
@@ -10976,7 +10984,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="250" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
         <v>42</v>
       </c>
@@ -11018,7 +11026,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="251" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
         <v>43</v>
       </c>
@@ -11060,7 +11068,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="252" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
         <v>41</v>
       </c>
@@ -11102,7 +11110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="253" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
         <v>44</v>
       </c>
@@ -11144,7 +11152,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="254" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
         <v>38</v>
       </c>
@@ -11186,7 +11194,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="255" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
         <v>42</v>
       </c>
@@ -11228,7 +11236,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="256" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
         <v>44</v>
       </c>
@@ -11270,7 +11278,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="257" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A257" s="1" t="s">
         <v>45</v>
       </c>
@@ -11312,7 +11320,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="258" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
         <v>41</v>
       </c>
@@ -11354,7 +11362,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="259" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
         <v>43</v>
       </c>
@@ -11396,7 +11404,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="260" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
         <v>44</v>
       </c>
@@ -11438,7 +11446,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="261" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A261" s="1" t="s">
         <v>45</v>
       </c>
@@ -11480,7 +11488,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="262" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
         <v>42</v>
       </c>
@@ -11522,7 +11530,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="263" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
         <v>41</v>
       </c>
@@ -11564,7 +11572,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="264" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
         <v>43</v>
       </c>
@@ -11606,7 +11614,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="265" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
         <v>38</v>
       </c>
@@ -11648,7 +11656,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="266" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
         <v>44</v>
       </c>
@@ -11690,7 +11698,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="267" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
         <v>41</v>
       </c>
@@ -11732,7 +11740,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="268" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
         <v>43</v>
       </c>
@@ -11774,7 +11782,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="269" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
         <v>42</v>
       </c>
@@ -11816,7 +11824,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="270" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A270" s="1" t="s">
         <v>45</v>
       </c>
@@ -11858,7 +11866,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="271" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
         <v>44</v>
       </c>
@@ -11900,7 +11908,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="272" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
         <v>41</v>
       </c>
@@ -11942,7 +11950,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="273" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
         <v>46</v>
       </c>
@@ -11984,7 +11992,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="274" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
         <v>42</v>
       </c>
@@ -12026,7 +12034,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="275" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
         <v>43</v>
       </c>
@@ -12068,7 +12076,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="276" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A276" s="1" t="s">
         <v>45</v>
       </c>
@@ -12110,7 +12118,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="277" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
         <v>44</v>
       </c>
@@ -12152,7 +12160,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="278" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
         <v>43</v>
       </c>
@@ -12194,7 +12202,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="279" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A279" s="1" t="s">
         <v>45</v>
       </c>
@@ -12236,7 +12244,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="280" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
         <v>42</v>
       </c>
@@ -12278,7 +12286,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="281" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A281" s="1" t="s">
         <v>45</v>
       </c>
@@ -12320,7 +12328,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="282" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
         <v>46</v>
       </c>
@@ -12362,7 +12370,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="283" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
         <v>47</v>
       </c>
@@ -12404,7 +12412,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="284" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
         <v>47</v>
       </c>
@@ -12446,7 +12454,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="285" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
         <v>47</v>
       </c>
@@ -12488,7 +12496,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="286" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
         <v>47</v>
       </c>
@@ -12530,7 +12538,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="287" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
         <v>48</v>
       </c>
@@ -12572,7 +12580,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="288" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
         <v>46</v>
       </c>
@@ -12614,7 +12622,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="289" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
         <v>47</v>
       </c>
@@ -12656,7 +12664,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="290" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
         <v>48</v>
       </c>
@@ -12698,7 +12706,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="291" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
         <v>47</v>
       </c>
@@ -12740,7 +12748,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="292" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
         <v>48</v>
       </c>
@@ -12782,7 +12790,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="293" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
         <v>47</v>
       </c>
@@ -12824,7 +12832,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="294" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
         <v>48</v>
       </c>
@@ -12866,7 +12874,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="295" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
         <v>46</v>
       </c>
@@ -12908,7 +12916,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="296" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
         <v>47</v>
       </c>
@@ -12950,7 +12958,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="297" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
         <v>48</v>
       </c>
@@ -12992,7 +13000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="298" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
         <v>47</v>
       </c>
@@ -13034,7 +13042,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="299" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
         <v>48</v>
       </c>
@@ -13076,7 +13084,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="300" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
         <v>48</v>
       </c>
@@ -13118,7 +13126,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="301" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
         <v>48</v>
       </c>
@@ -13160,7 +13168,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="302" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A302" t="s">
         <v>48</v>
       </c>
@@ -13202,7 +13210,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="303" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A303" t="s">
         <v>49</v>
       </c>
@@ -13244,7 +13252,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="304" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A304" t="s">
         <v>49</v>
       </c>
@@ -13286,7 +13294,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="305" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A305" t="s">
         <v>49</v>
       </c>
@@ -13328,7 +13336,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="306" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A306" t="s">
         <v>50</v>
       </c>
@@ -13370,7 +13378,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="307" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
         <v>46</v>
       </c>
@@ -13412,7 +13420,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="308" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A308" t="s">
         <v>51</v>
       </c>
@@ -13454,7 +13462,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="309" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A309" t="s">
         <v>49</v>
       </c>
@@ -13496,7 +13504,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="310" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A310" t="s">
         <v>46</v>
       </c>
@@ -13538,7 +13546,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="311" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A311" t="s">
         <v>49</v>
       </c>
@@ -13580,7 +13588,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="312" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A312" t="s">
         <v>52</v>
       </c>
@@ -13622,7 +13630,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="313" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A313" t="s">
         <v>51</v>
       </c>
@@ -13664,7 +13672,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="314" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A314" t="s">
         <v>49</v>
       </c>
@@ -13706,7 +13714,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="315" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A315" t="s">
         <v>46</v>
       </c>
@@ -13748,7 +13756,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="316" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A316" t="s">
         <v>50</v>
       </c>
@@ -13790,7 +13798,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="317" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
         <v>52</v>
       </c>
@@ -13832,7 +13840,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="318" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A318" t="s">
         <v>49</v>
       </c>
@@ -13874,7 +13882,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="319" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A319" t="s">
         <v>51</v>
       </c>
@@ -13916,7 +13924,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="320" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A320" t="s">
         <v>52</v>
       </c>
@@ -13958,7 +13966,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="321" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A321" t="s">
         <v>50</v>
       </c>
@@ -14000,7 +14008,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="322" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A322" t="s">
         <v>49</v>
       </c>
@@ -14042,7 +14050,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="323" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A323" t="s">
         <v>46</v>
       </c>
@@ -14084,7 +14092,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="324" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A324" t="s">
         <v>52</v>
       </c>
@@ -14126,7 +14134,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="325" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
         <v>51</v>
       </c>
@@ -14168,7 +14176,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="326" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A326" t="s">
         <v>49</v>
       </c>
@@ -14210,7 +14218,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="327" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A327" t="s">
         <v>50</v>
       </c>
@@ -14252,7 +14260,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="328" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A328" t="s">
         <v>52</v>
       </c>
@@ -14294,7 +14302,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="329" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A329" t="s">
         <v>51</v>
       </c>
@@ -14336,7 +14344,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="330" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A330" t="s">
         <v>50</v>
       </c>
@@ -14378,7 +14386,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="331" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A331" t="s">
         <v>46</v>
       </c>
@@ -14420,7 +14428,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="332" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A332" t="s">
         <v>52</v>
       </c>
@@ -14462,7 +14470,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="333" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A333" t="s">
         <v>50</v>
       </c>
@@ -14504,7 +14512,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="334" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A334" t="s">
         <v>51</v>
       </c>
@@ -14546,7 +14554,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="335" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A335" t="s">
         <v>52</v>
       </c>
@@ -14588,7 +14596,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="336" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A336" t="s">
         <v>51</v>
       </c>
@@ -14630,7 +14638,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="337" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A337" t="s">
         <v>50</v>
       </c>
@@ -14672,7 +14680,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="338" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A338" t="s">
         <v>52</v>
       </c>
@@ -14714,7 +14722,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="339" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A339" t="s">
         <v>50</v>
       </c>
@@ -14756,7 +14764,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="340" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A340" t="s">
         <v>52</v>
       </c>
@@ -14798,7 +14806,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="341" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A341" t="s">
         <v>51</v>
       </c>
@@ -14840,7 +14848,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="342" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A342" t="s">
         <v>51</v>
       </c>
@@ -14882,7 +14890,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="343" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A343" t="s">
         <v>50</v>
       </c>
@@ -14926,6 +14934,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -14935,7 +14944,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -14947,7 +14956,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>